<commit_message>
added the second step for data renaming
</commit_message>
<xml_diff>
--- a/docs/columnnames.xlsx
+++ b/docs/columnnames.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>Generation</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Use all info to make a new name eg., G1mmqupar. Variables that are not needed are left blank</t>
+  </si>
+  <si>
+    <t>use the &amp; option in excel to merge all cells e.g. C1&amp;C2</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,6 +640,9 @@
       <c r="E5" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
Changed the output of the create_codebook to excel
</commit_message>
<xml_diff>
--- a/docs/columnnames.xlsx
+++ b/docs/columnnames.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Generation</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>use the &amp; option in excel to merge all cells e.g. C1&amp;C2</t>
+  </si>
+  <si>
+    <t>new_value_label</t>
+  </si>
+  <si>
+    <t>If novalue labels are provided, give a label.provide the value and the label, seperated by comma, similar to the value_label column</t>
   </si>
 </sst>
 </file>
@@ -531,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,10 +552,11 @@
     <col min="5" max="5" width="25.1796875" customWidth="1"/>
     <col min="6" max="6" width="13.90625" customWidth="1"/>
     <col min="7" max="7" width="22.90625" customWidth="1"/>
-    <col min="8" max="8" width="17.1796875" customWidth="1"/>
+    <col min="8" max="9" width="17.1796875" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,10 +582,13 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -604,10 +614,13 @@
         <v>41</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -624,7 +637,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -644,7 +657,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -661,7 +674,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -673,7 +686,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -685,7 +698,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
@@ -696,7 +709,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C10" s="1" t="s">
         <v>36</v>
       </c>
@@ -707,7 +720,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
@@ -715,7 +728,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
@@ -723,7 +736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
@@ -731,17 +744,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>